<commit_message>
Thêm activity vào Quản lí danh mục
</commit_message>
<xml_diff>
--- a/Phân tích/UseCases/3. Quản lí danh mục.xlsx
+++ b/Phân tích/UseCases/3. Quản lí danh mục.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\CNPM\Phân tích\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05497DD1-B57C-4C35-B20F-A1208BC9C341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40403CD6-2CC7-4111-AC4F-F6F60F17067B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04392538-DB61-43EC-AFA3-E88B6D995574}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{04392538-DB61-43EC-AFA3-E88B6D995574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -318,11 +318,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -342,27 +360,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -380,6 +377,54 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,6 +441,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3000375</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>113300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D34ECD2-BFC8-4004-8FB0-DE1B9D6F2151}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="6343650"/>
+          <a:ext cx="6772275" cy="8000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,65 +789,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E5EAC9-BCA6-4B31-A937-E7944D29B1E5}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="15"/>
-    </row>
-    <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -764,162 +858,382 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="33" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="33" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="15"/>
-    </row>
-    <row r="23" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="8"/>
       <c r="E23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="9">
         <v>44159</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="22"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="25"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="25"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="25"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="25"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="25"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="25"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="25"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="25"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="25"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="25"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="25"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="25"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="25"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="25"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="25"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="25"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="25"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="25"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="25"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="25"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="23"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="23"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="25"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="25"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="26"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="19">
+    <mergeCell ref="A26:C69"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:C16"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
@@ -927,12 +1241,14 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:C16"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>